<commit_message>
raindrops, cite search improved
</commit_message>
<xml_diff>
--- a/dynamic_context_server/ref/AR-70-38_files/AR-70-38.xlsx
+++ b/dynamic_context_server/ref/AR-70-38_files/AR-70-38.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Height or Elevation</t>
   </si>
@@ -192,9 +192,6 @@
     <t>exp</t>
   </si>
   <si>
-    <t>entroplet</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -214,6 +211,33 @@
   </si>
   <si>
     <t xml:space="preserve">Table 2-8. Drop Diameter Range (mm) </t>
+  </si>
+  <si>
+    <t>Model has 99.5% of drops with mean size of 0.5 mm, and 0.5% with mean size 1.0 mm</t>
+  </si>
+  <si>
+    <t>Exponential model produces the distribution</t>
+  </si>
+  <si>
+    <t>1/mean</t>
+  </si>
+  <si>
+    <t>1/mean1</t>
+  </si>
+  <si>
+    <t>%mean</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>combo</t>
+  </si>
+  <si>
+    <t>histogram</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
@@ -286,7 +310,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +326,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF20B2AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -394,6 +472,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,12 +488,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +543,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38127819548872183"/>
-          <c:y val="1.532567049808429E-2"/>
+          <c:x val="0.38127819548872188"/>
+          <c:y val="1.5325670498084294E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -469,8 +556,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.24136351706036746"/>
           <c:y val="5.0925925925925923E-2"/>
-          <c:w val="0.6702073490813647"/>
-          <c:h val="0.71640419947506562"/>
+          <c:w val="0.67020734908136459"/>
+          <c:h val="0.71640419947506551"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -621,11 +708,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="110453888"/>
-        <c:axId val="99713408"/>
+        <c:axId val="152059264"/>
+        <c:axId val="152127360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110453888"/>
+        <c:axId val="152059264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,19 +738,19 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="1.7529256211394628E-2"/>
-              <c:y val="0.18942890759344738"/>
+              <c:y val="0.18942890759344744"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99713408"/>
+        <c:crossAx val="152127360"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99713408"/>
+        <c:axId val="152127360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -689,7 +776,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110453888"/>
+        <c:crossAx val="152059264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -700,9 +787,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.67439938428749047"/>
-          <c:y val="0.20507587413642261"/>
-          <c:w val="0.23082726501292603"/>
+          <c:x val="0.67439938428749069"/>
+          <c:y val="0.20507587413642264"/>
+          <c:w val="0.23082726501292605"/>
           <c:h val="0.15711527438380546"/>
         </c:manualLayout>
       </c:layout>
@@ -721,7 +808,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -732,15 +819,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1097,26 +1184,26 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="1" t="s">
@@ -1262,10 +1349,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" ht="27.75" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -1320,7 +1407,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1329,15 +1416,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="A1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -1364,7 +1451,7 @@
     </row>
     <row r="3" spans="1:9" ht="47.25">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8">
         <v>2626</v>
@@ -1382,56 +1469,59 @@
         <v>1</v>
       </c>
       <c r="G3" s="8"/>
-      <c r="I3">
-        <v>0.98599999999999999</v>
-      </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="14">
+      <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10">
         <f>+$G$7</f>
         <v>2617.4408510083717</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <f>+$G$8</f>
         <v>342.0961097050897</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <f>+$G$9</f>
         <v>45.554505437617472</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <f>+$G$10</f>
         <v>6.3718712639070363</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="10">
         <f>+$G$11</f>
         <v>1.0000646561675552</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="10">
         <f>+$G$12</f>
         <v>0.1938300861431812</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="B5">
+      <c r="A5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="20">
         <v>9000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="23">
         <v>2.1</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="21">
         <v>8643.0000000000036</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="15">
         <v>2.0453672195498638</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="17">
         <v>1.0038377298476968</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="18">
         <v>0.99515546875000571</v>
       </c>
     </row>
@@ -1439,34 +1529,46 @@
       <c r="A6">
         <v>0.1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
-        <v>33</v>
+      <c r="C6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="22">
         <f>+$B$5*EXP(-$C$5*$A7)</f>
         <v>9000</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="22">
         <f>+B$12-B$21</f>
         <v>2673.6481833552448</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="16">
         <f>+$F$5*($I$5*EXP(-$G$5*$A7)+(1-$I$5)*EXP(-$H$5*$A7))</f>
         <v>8643.0000000000036</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="16">
         <f>+F$12-F$21</f>
         <v>2617.4408510083717</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="19">
         <f>+(ABS(LN($B$3/$G$7))+ABS(LN($C$3/$G$8))+ABS(LN($D$3/$G$9)))</f>
         <v>1.5792733893715449E-2</v>
       </c>
@@ -1476,23 +1578,23 @@
         <f>+$A7+$A$6</f>
         <v>0.1</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="22">
         <f t="shared" ref="B8:B71" si="0">+$B$5*EXP(-$C$5*$A8)</f>
         <v>7295.258213731684</v>
       </c>
-      <c r="D8">
+      <c r="C8" s="22">
         <f>+B$22-B$31</f>
         <v>327.40540693875676</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="16">
         <f t="shared" ref="F8:F71" si="1">+$F$5*($I$5*EXP(-$G$5*$A8)+(1-$I$5)*EXP(-$H$5*$A8))</f>
         <v>7048.005482655999</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="16">
         <f>+F$22-F$31</f>
         <v>342.0961097050897</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="19">
         <f>+(ABS(LN($E$3/$G$10))+ABS(LN($F$3/$G$11)))</f>
         <v>6.0198373288670941E-2</v>
       </c>
@@ -1502,23 +1604,23 @@
         <f t="shared" ref="A9:A71" si="2">+$A8+$A$6</f>
         <v>0.2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="22">
         <f t="shared" si="0"/>
         <v>5913.4213783355108</v>
       </c>
-      <c r="D9">
+      <c r="C9" s="22">
         <f>+B$32-B$41</f>
         <v>40.092896724434183</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="16">
         <f t="shared" si="1"/>
         <v>5747.6875932708699</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="16">
         <f>+F$32-F$41</f>
         <v>45.554505437617472</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="19">
         <f>+$I$7+$I$8</f>
         <v>7.5991107182386386E-2</v>
       </c>
@@ -1528,41 +1630,44 @@
         <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="22">
         <f t="shared" si="0"/>
         <v>4793.3262090620747</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="22">
         <f>+B$42-B$51</f>
         <v>4.909632931189873</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="16">
         <f t="shared" si="1"/>
         <v>4687.5726389446272</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="16">
         <f>+F$42-F$51</f>
         <v>6.3718712639070363</v>
       </c>
+      <c r="I10" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="22">
         <f t="shared" si="0"/>
         <v>3885.3947108617172</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="22">
         <f>+B$52-B$61</f>
         <v>0.60121611278673126</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>3823.2599446243698</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="16">
         <f>+F$52-F$61</f>
         <v>1.0000646561675552</v>
       </c>
@@ -1572,19 +1677,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="22">
         <f t="shared" si="0"/>
         <v>3149.4397420003979</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="22">
         <f>+B$62-B$71</f>
         <v>7.3622777780005588E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="16">
         <f t="shared" si="1"/>
         <v>3118.5589064534852</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="16">
         <f>+F$62-F$71</f>
         <v>0.1938300861431812</v>
       </c>
@@ -1594,13 +1699,19 @@
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="22">
         <f t="shared" si="0"/>
         <v>2552.8862384979334</v>
       </c>
-      <c r="F13">
+      <c r="C13" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="16">
         <f t="shared" si="1"/>
         <v>2543.9706142555092</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1608,11 +1719,11 @@
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="22">
         <f t="shared" si="0"/>
         <v>2069.3293666805148</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="16">
         <f t="shared" si="1"/>
         <v>2075.4503092557779</v>
       </c>
@@ -1622,13 +1733,16 @@
         <f t="shared" si="2"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="22">
         <f t="shared" si="0"/>
         <v>1677.3657843546898</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="16">
         <f t="shared" si="1"/>
         <v>1693.3987320618935</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1636,13 +1750,16 @@
         <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="22">
         <f t="shared" si="0"/>
         <v>1359.6462795273378</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="16">
         <f t="shared" si="1"/>
         <v>1381.8400242106973</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1650,11 +1767,11 @@
         <f t="shared" si="2"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="22">
         <f t="shared" si="0"/>
         <v>1102.1078542768375</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="16">
         <f t="shared" si="1"/>
         <v>1127.7516776048171</v>
       </c>
@@ -1664,11 +1781,11 @@
         <f t="shared" si="2"/>
         <v>1.0999999999999999</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="22">
         <f t="shared" si="0"/>
         <v>893.35126403681124</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="16">
         <f t="shared" si="1"/>
         <v>920.5184086550056</v>
       </c>
@@ -1678,11 +1795,11 @@
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="22">
         <f t="shared" si="0"/>
         <v>724.13646074579196</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="16">
         <f t="shared" si="1"/>
         <v>751.48703585390717</v>
       </c>
@@ -1692,11 +1809,11 @@
         <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="22">
         <f t="shared" si="0"/>
         <v>586.97360701314744</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="16">
         <f t="shared" si="1"/>
         <v>613.60367920951342</v>
       </c>
@@ -1706,11 +1823,11 @@
         <f t="shared" si="2"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="22">
         <f t="shared" si="0"/>
         <v>475.79155864515303</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="16">
         <f t="shared" si="1"/>
         <v>501.11805544511355</v>
       </c>
@@ -1720,11 +1837,11 @@
         <f t="shared" si="2"/>
         <v>1.5000000000000002</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="22">
         <f t="shared" si="0"/>
         <v>385.6691418033613</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="16">
         <f t="shared" si="1"/>
         <v>409.34245918748172</v>
       </c>
@@ -1734,11 +1851,11 @@
         <f t="shared" si="2"/>
         <v>1.6000000000000003</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="22">
         <f t="shared" si="0"/>
         <v>312.61733050264684</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="16">
         <f t="shared" si="1"/>
         <v>334.45531574446397</v>
       </c>
@@ -1748,11 +1865,11 @@
         <f t="shared" si="2"/>
         <v>1.7000000000000004</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="22">
         <f t="shared" si="0"/>
         <v>253.40268312270064</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="16">
         <f t="shared" si="1"/>
         <v>273.34106187590294</v>
       </c>
@@ -1762,11 +1879,11 @@
         <f t="shared" si="2"/>
         <v>1.8000000000000005</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="22">
         <f t="shared" si="0"/>
         <v>205.40422282583654</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="16">
         <f t="shared" si="1"/>
         <v>223.45963572305229</v>
       </c>
@@ -1776,11 +1893,11 @@
         <f t="shared" si="2"/>
         <v>1.9000000000000006</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="22">
         <f t="shared" si="0"/>
         <v>166.49742707837297</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="16">
         <f t="shared" si="1"/>
         <v>182.74009978934291</v>
       </c>
@@ -1790,11 +1907,11 @@
         <f t="shared" si="2"/>
         <v>2.0000000000000004</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="22">
         <f t="shared" si="0"/>
         <v>134.96019138429921</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="16">
         <f t="shared" si="1"/>
         <v>149.49393372788859</v>
       </c>
@@ -1804,11 +1921,11 @@
         <f t="shared" si="2"/>
         <v>2.1000000000000005</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="22">
         <f t="shared" si="0"/>
         <v>109.39660496923432</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="16">
         <f t="shared" si="1"/>
         <v>122.34435920698147</v>
       </c>
@@ -1818,11 +1935,11 @@
         <f t="shared" si="2"/>
         <v>2.2000000000000006</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="22">
         <f t="shared" si="0"/>
         <v>88.675164550685153</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="16">
         <f t="shared" si="1"/>
         <v>100.16873194777504</v>
       </c>
@@ -1832,11 +1949,11 @@
         <f t="shared" si="2"/>
         <v>2.3000000000000007</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="22">
         <f t="shared" si="0"/>
         <v>71.878691393599397</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="16">
         <f t="shared" si="1"/>
         <v>82.051584402107352</v>
       </c>
@@ -1846,11 +1963,11 @@
         <f t="shared" si="2"/>
         <v>2.4000000000000008</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="22">
         <f t="shared" si="0"/>
         <v>58.263734864604544</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="16">
         <f t="shared" si="1"/>
         <v>67.246349482392034</v>
       </c>
@@ -1860,11 +1977,11 @@
         <f t="shared" si="2"/>
         <v>2.5000000000000009</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="22">
         <f t="shared" si="0"/>
         <v>47.227665592632377</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="16">
         <f t="shared" si="1"/>
         <v>55.144160031136281</v>
       </c>
@@ -1874,11 +1991,11 @@
         <f t="shared" si="2"/>
         <v>2.600000000000001</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="22">
         <f t="shared" si="0"/>
         <v>38.282001703336029</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="16">
         <f t="shared" si="1"/>
         <v>45.248415616031707</v>
       </c>
@@ -1888,11 +2005,11 @@
         <f t="shared" si="2"/>
         <v>2.7000000000000011</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="22">
         <f t="shared" si="0"/>
         <v>31.030787484928055</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="16">
         <f t="shared" si="1"/>
         <v>37.154050220374373</v>
       </c>
@@ -1902,11 +2019,11 @@
         <f t="shared" si="2"/>
         <v>2.8000000000000012</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="22">
         <f t="shared" si="0"/>
         <v>25.153067475331525</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="16">
         <f t="shared" si="1"/>
         <v>30.530631625230761</v>
       </c>
@@ -1916,11 +2033,11 @@
         <f t="shared" si="2"/>
         <v>2.9000000000000012</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="22">
         <f t="shared" si="0"/>
         <v>20.388680233328841</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="16">
         <f t="shared" si="1"/>
         <v>25.108584027872144</v>
       </c>
@@ -1930,11 +2047,11 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000013</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="22">
         <f t="shared" si="0"/>
         <v>16.526742993260104</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="16">
         <f t="shared" si="1"/>
         <v>20.667956457845957</v>
       </c>
@@ -1944,11 +2061,11 @@
         <f t="shared" si="2"/>
         <v>3.1000000000000014</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="22">
         <f t="shared" si="0"/>
         <v>13.396317507534816</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="16">
         <f t="shared" si="1"/>
         <v>17.029266336881719</v>
       </c>
@@ -1958,11 +2075,11 @@
         <f t="shared" si="2"/>
         <v>3.2000000000000015</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="22">
         <f t="shared" si="0"/>
         <v>10.858843925622326</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="16">
         <f t="shared" si="1"/>
         <v>14.046034563693896</v>
       </c>
@@ -1972,11 +2089,11 @@
         <f t="shared" si="2"/>
         <v>3.3000000000000016</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="22">
         <f t="shared" si="0"/>
         <v>8.80200781555852</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="16">
         <f t="shared" si="1"/>
         <v>11.598699442648041</v>
       </c>
@@ -1986,11 +2103,11 @@
         <f t="shared" si="2"/>
         <v>3.4000000000000017</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="22">
         <f t="shared" si="0"/>
         <v>7.13476886819819</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="16">
         <f t="shared" si="1"/>
         <v>9.5896545935188087</v>
       </c>
@@ -2000,11 +2117,11 @@
         <f t="shared" si="2"/>
         <v>3.5000000000000018</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="22">
         <f t="shared" si="0"/>
         <v>5.7833312431999957</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="16">
         <f t="shared" si="1"/>
         <v>7.9392031047933047</v>
       </c>
@@ -2014,11 +2131,11 @@
         <f t="shared" si="2"/>
         <v>3.6000000000000019</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="22">
         <f t="shared" si="0"/>
         <v>4.6878771949650933</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="16">
         <f t="shared" si="1"/>
         <v>6.5822586029264745</v>
       </c>
@@ -2028,11 +2145,11 @@
         <f t="shared" si="2"/>
         <v>3.700000000000002</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="22">
         <f t="shared" si="0"/>
         <v>3.799919401281616</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="16">
         <f t="shared" si="1"/>
         <v>5.4656552165804628</v>
       </c>
@@ -2042,11 +2159,11 @@
         <f t="shared" si="2"/>
         <v>3.800000000000002</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="22">
         <f t="shared" si="0"/>
         <v>3.0801548026353407</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="16">
         <f t="shared" si="1"/>
         <v>4.5459539319677962</v>
       </c>
@@ -2056,11 +2173,11 @@
         <f t="shared" si="2"/>
         <v>3.9000000000000021</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="22">
         <f t="shared" si="0"/>
         <v>2.4967249581656183</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="16">
         <f t="shared" si="1"/>
         <v>3.7876536337545681</v>
       </c>
@@ -2070,11 +2187,11 @@
         <f t="shared" si="2"/>
         <v>4.0000000000000018</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="22">
         <f t="shared" si="0"/>
         <v>2.0238059176096264</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="16">
         <f t="shared" si="1"/>
         <v>3.161732078294746</v>
       </c>
@@ -2084,11 +2201,11 @@
         <f t="shared" si="2"/>
         <v>4.1000000000000014</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="22">
         <f t="shared" si="0"/>
         <v>1.6404651937156032</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="16">
         <f t="shared" si="1"/>
         <v>2.6444558635683988</v>
       </c>
@@ -2098,11 +2215,11 @@
         <f t="shared" si="2"/>
         <v>4.2000000000000011</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="22">
         <f t="shared" si="0"/>
         <v>1.3297352420883004</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="16">
         <f t="shared" si="1"/>
         <v>2.216409722829594</v>
       </c>
@@ -2112,11 +2229,11 @@
         <f t="shared" si="2"/>
         <v>4.3000000000000007</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="22">
         <f t="shared" si="0"/>
         <v>1.0778624385481301</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="16">
         <f t="shared" si="1"/>
         <v>1.8617046491493627</v>
       </c>
@@ -2126,11 +2243,11 @@
         <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="22">
         <f t="shared" si="0"/>
         <v>0.87369831201012249</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="16">
         <f t="shared" si="1"/>
         <v>1.5673318408862686</v>
       </c>
@@ -2140,11 +2257,11 @@
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="22">
         <f t="shared" si="0"/>
         <v>0.70820608744615099</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="16">
         <f t="shared" si="1"/>
         <v>1.32263555752216</v>
       </c>
@@ -2154,11 +2271,11 @@
         <f t="shared" si="2"/>
         <v>4.5999999999999996</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="22">
         <f t="shared" si="0"/>
         <v>0.57406069738403531</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="16">
         <f t="shared" si="1"/>
         <v>1.1188829470994219</v>
       </c>
@@ -2168,11 +2285,11 @@
         <f t="shared" si="2"/>
         <v>4.6999999999999993</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="22">
         <f t="shared" si="0"/>
         <v>0.46532455753015839</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="16">
         <f t="shared" si="1"/>
         <v>0.94891295920724683</v>
       </c>
@@ -2182,11 +2299,11 @@
         <f t="shared" si="2"/>
         <v>4.7999999999999989</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="22">
         <f t="shared" si="0"/>
         <v>0.37718475559699477</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="16">
         <f t="shared" si="1"/>
         <v>0.806849761041872</v>
       </c>
@@ -2196,11 +2313,11 @@
         <f t="shared" si="2"/>
         <v>4.8999999999999986</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="22">
         <f t="shared" si="0"/>
         <v>0.30574002070703954</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="16">
         <f t="shared" si="1"/>
         <v>0.68786876703118738</v>
       </c>
@@ -2210,11 +2327,11 @@
         <f t="shared" si="2"/>
         <v>4.9999999999999982</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="22">
         <f t="shared" si="0"/>
         <v>0.2478280441477253</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="16">
         <f t="shared" si="1"/>
         <v>0.58800558777091261</v>
       </c>
@@ -2224,11 +2341,11 @@
         <f t="shared" si="2"/>
         <v>5.0999999999999979</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="22">
         <f t="shared" si="0"/>
         <v>0.20088550829575033</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="16">
         <f t="shared" si="1"/>
         <v>0.50399999359108238</v>
       </c>
@@ -2238,11 +2355,11 @@
         <f t="shared" si="2"/>
         <v>5.1999999999999975</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="22">
         <f t="shared" si="0"/>
         <v>0.16283462826824871</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="16">
         <f t="shared" si="1"/>
         <v>0.43316844696296092</v>
       </c>
@@ -2252,11 +2369,11 @@
         <f t="shared" si="2"/>
         <v>5.2999999999999972</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="22">
         <f t="shared" si="0"/>
         <v>0.1319911843726542</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="16">
         <f t="shared" si="1"/>
         <v>0.37329994730232258</v>
       </c>
@@ -2266,11 +2383,11 @@
         <f t="shared" si="2"/>
         <v>5.3999999999999968</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="22">
         <f t="shared" si="0"/>
         <v>0.10698997465941976</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="16">
         <f t="shared" si="1"/>
         <v>0.3225709013546047</v>
       </c>
@@ -2280,11 +2397,11 @@
         <f t="shared" si="2"/>
         <v>5.4999999999999964</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="22">
         <f t="shared" si="0"/>
         <v>8.6724387935675273E-2</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="16">
         <f t="shared" si="1"/>
         <v>0.27947552287576627</v>
       </c>
@@ -2294,11 +2411,11 @@
         <f t="shared" si="2"/>
         <v>5.5999999999999961</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="22">
         <f t="shared" si="0"/>
         <v>7.0297422602065396E-2</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="16">
         <f t="shared" si="1"/>
         <v>0.24276890985459815</v>
       </c>
@@ -2308,11 +2425,11 @@
         <f t="shared" si="2"/>
         <v>5.6999999999999957</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="22">
         <f t="shared" si="0"/>
         <v>5.6981983293542822E-2</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="16">
         <f t="shared" si="1"/>
         <v>0.21142047304130335</v>
       </c>
@@ -2322,11 +2439,11 @@
         <f t="shared" si="2"/>
         <v>5.7999999999999954</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="22">
         <f t="shared" si="0"/>
         <v>4.6188697961882255E-2</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="16">
         <f t="shared" si="1"/>
         <v>0.18457581804780607</v>
       </c>
@@ -2336,11 +2453,11 @@
         <f t="shared" si="2"/>
         <v>5.899999999999995</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="22">
         <f t="shared" si="0"/>
         <v>3.7439830909777073E-2</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="16">
         <f t="shared" si="1"/>
         <v>0.16152553269536163</v>
       </c>
@@ -2350,11 +2467,11 @@
         <f t="shared" si="2"/>
         <v>5.9999999999999947</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="22">
         <f t="shared" si="0"/>
         <v>3.0348137107252985E-2</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="16">
         <f t="shared" si="1"/>
         <v>0.14167961621802541</v>
       </c>
@@ -2364,11 +2481,11 @@
         <f t="shared" si="2"/>
         <v>6.0999999999999943</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="22">
         <f t="shared" si="0"/>
         <v>2.4599721833682538E-2</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="16">
         <f t="shared" si="1"/>
         <v>0.1245465192982609</v>
       </c>
@@ -2378,11 +2495,11 @@
         <f t="shared" si="2"/>
         <v>6.199999999999994</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="22">
         <f t="shared" si="0"/>
         <v>1.9940146973631927E-2</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="16">
         <f t="shared" si="1"/>
         <v>0.10971595342329599</v>
       </c>
@@ -2392,11 +2509,11 @@
         <f t="shared" si="2"/>
         <v>6.2999999999999936</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="22">
         <f t="shared" si="0"/>
         <v>1.6163168999156131E-2</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="16">
         <f t="shared" si="1"/>
         <v>9.6844782622840131E-2</v>
       </c>
@@ -2406,11 +2523,11 @@
         <f t="shared" si="2"/>
         <v>6.3999999999999932</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="22">
         <f t="shared" si="0"/>
         <v>1.3101610155669687E-2</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="16">
         <f t="shared" si="1"/>
         <v>8.5645436732585067E-2</v>
       </c>

</xml_diff>

<commit_message>
added a unit scaling function
</commit_message>
<xml_diff>
--- a/dynamic_context_server/ref/AR-70-38_files/AR-70-38.xlsx
+++ b/dynamic_context_server/ref/AR-70-38_files/AR-70-38.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="19935" windowHeight="10575" activeTab="2"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Height or Elevation</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>mean1</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -687,22 +693,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2617.4408510083717</c:v>
+                  <c:v>2617.4684326269048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>342.0961097050897</c:v>
+                  <c:v>342.14061496928451</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.554505437617472</c:v>
+                  <c:v>45.57526400696117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3718712639070363</c:v>
+                  <c:v>6.3800540272725623</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0000646561675552</c:v>
+                  <c:v>1.0031378094521939</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1938300861431812</c:v>
+                  <c:v>0.19496592970254101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,6 +1181,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1336,6 +1343,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1404,10 +1412,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I71"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1415,7 +1424,7 @@
     <col min="2" max="7" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
@@ -1426,7 +1435,7 @@
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1449,7 +1458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="47.25">
+    <row r="3" spans="1:12" ht="47.25">
       <c r="A3" s="7" t="s">
         <v>34</v>
       </c>
@@ -1470,36 +1479,36 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="10">
         <f>+$G$7</f>
-        <v>2617.4408510083717</v>
+        <v>2617.4684326269048</v>
       </c>
       <c r="C4" s="10">
         <f>+$G$8</f>
-        <v>342.0961097050897</v>
+        <v>342.14061496928451</v>
       </c>
       <c r="D4" s="10">
         <f>+$G$9</f>
-        <v>45.554505437617472</v>
+        <v>45.57526400696117</v>
       </c>
       <c r="E4" s="10">
         <f>+$G$10</f>
-        <v>6.3718712639070363</v>
+        <v>6.3800540272725623</v>
       </c>
       <c r="F4" s="10">
         <f>+$G$11</f>
-        <v>1.0000646561675552</v>
+        <v>1.0031378094521939</v>
       </c>
       <c r="G4" s="10">
         <f>+$G$12</f>
-        <v>0.1938300861431812</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.19496592970254101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
@@ -1522,10 +1531,10 @@
         <v>1.0038377298476968</v>
       </c>
       <c r="I5" s="18">
-        <v>0.99515546875000571</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.99509999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>0.1</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1566,14 +1575,14 @@
       </c>
       <c r="G7" s="16">
         <f>+F$12-F$21</f>
-        <v>2617.4408510083717</v>
+        <v>2617.4684326269048</v>
       </c>
       <c r="I7" s="19">
         <f>+(ABS(LN($B$3/$G$7))+ABS(LN($C$3/$G$8))+ABS(LN($D$3/$G$9)))</f>
-        <v>1.5792733893715449E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>1.6367866274000758E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <f>+$A7+$A$6</f>
         <v>0.1</v>
@@ -1588,18 +1597,18 @@
       </c>
       <c r="F8" s="16">
         <f t="shared" ref="F8:F71" si="1">+$F$5*($I$5*EXP(-$G$5*$A8)+(1-$I$5)*EXP(-$H$5*$A8))</f>
-        <v>7048.005482655999</v>
+        <v>7048.0483738463536</v>
       </c>
       <c r="G8" s="16">
         <f>+F$22-F$31</f>
-        <v>342.0961097050897</v>
+        <v>342.14061496928451</v>
       </c>
       <c r="I8" s="19">
         <f>+(ABS(LN($E$3/$G$10))+ABS(LN($F$3/$G$11)))</f>
-        <v>6.0198373288670941E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>6.4549993119399907E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <f t="shared" ref="A9:A71" si="2">+$A8+$A$6</f>
         <v>0.2</v>
@@ -1614,18 +1623,18 @@
       </c>
       <c r="F9" s="16">
         <f t="shared" si="1"/>
-        <v>5747.6875932708699</v>
+        <v>5747.7613453179674</v>
       </c>
       <c r="G9" s="16">
         <f>+F$32-F$41</f>
-        <v>45.554505437617472</v>
+        <v>45.57526400696117</v>
       </c>
       <c r="I9" s="19">
         <f>+$I$7+$I$8</f>
-        <v>7.5991107182386386E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>8.0917859393400668E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
@@ -1640,17 +1649,17 @@
       </c>
       <c r="F10" s="16">
         <f t="shared" si="1"/>
-        <v>4687.5726389446272</v>
+        <v>4687.6678380864696</v>
       </c>
       <c r="G10" s="16">
         <f>+F$42-F$51</f>
-        <v>6.3718712639070363</v>
+        <v>6.3800540272725623</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>0.4</v>
@@ -1665,14 +1674,14 @@
       </c>
       <c r="F11" s="16">
         <f t="shared" si="1"/>
-        <v>3823.2599446243698</v>
+        <v>3823.3692723007607</v>
       </c>
       <c r="G11" s="16">
         <f>+F$52-F$61</f>
-        <v>1.0000646561675552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>1.0031378094521939</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -1687,14 +1696,14 @@
       </c>
       <c r="F12" s="16">
         <f t="shared" si="1"/>
-        <v>3118.5589064534852</v>
+        <v>3118.6767179457815</v>
       </c>
       <c r="G12" s="16">
         <f>+F$62-F$71</f>
-        <v>0.1938300861431812</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.19496592970254101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>0.6</v>
@@ -1708,13 +1717,13 @@
       </c>
       <c r="F13" s="16">
         <f t="shared" si="1"/>
-        <v>2543.9706142555092</v>
+        <v>2544.0925984957935</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>0.7</v>
@@ -1725,10 +1734,24 @@
       </c>
       <c r="F14" s="16">
         <f t="shared" si="1"/>
-        <v>2075.4503092557779</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>2075.5732144827812</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="15">
+        <f>1/G5</f>
+        <v>0.48890976174932343</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="17">
+        <f>1/H5</f>
+        <v>0.99617694201603768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>0.79999999999999993</v>
@@ -1739,13 +1762,13 @@
       </c>
       <c r="F15" s="16">
         <f t="shared" si="1"/>
-        <v>1693.3987320618935</v>
+        <v>1693.5201448647854</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>0.89999999999999991</v>
@@ -1756,7 +1779,7 @@
       </c>
       <c r="F16" s="16">
         <f t="shared" si="1"/>
-        <v>1381.8400242106973</v>
+        <v>1381.9581918330623</v>
       </c>
       <c r="H16" t="s">
         <v>37</v>
@@ -1773,7 +1796,7 @@
       </c>
       <c r="F17" s="16">
         <f t="shared" si="1"/>
-        <v>1127.7516776048171</v>
+        <v>1127.8653652786077</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1787,7 +1810,7 @@
       </c>
       <c r="F18" s="16">
         <f t="shared" si="1"/>
-        <v>920.5184086550056</v>
+        <v>920.62678527843525</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1801,7 +1824,7 @@
       </c>
       <c r="F19" s="16">
         <f t="shared" si="1"/>
-        <v>751.48703585390717</v>
+        <v>751.58958258370717</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1815,7 +1838,7 @@
       </c>
       <c r="F20" s="16">
         <f t="shared" si="1"/>
-        <v>613.60367920951342</v>
+        <v>613.7001165601398</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1829,7 +1852,7 @@
       </c>
       <c r="F21" s="16">
         <f t="shared" si="1"/>
-        <v>501.11805544511355</v>
+        <v>501.20828531887662</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1843,7 +1866,7 @@
       </c>
       <c r="F22" s="16">
         <f t="shared" si="1"/>
-        <v>409.34245918748172</v>
+        <v>409.42651893563635</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1857,7 +1880,7 @@
       </c>
       <c r="F23" s="16">
         <f t="shared" si="1"/>
-        <v>334.45531574446397</v>
+        <v>334.53334190890388</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1871,7 +1894,7 @@
       </c>
       <c r="F24" s="16">
         <f t="shared" si="1"/>
-        <v>273.34106187590294</v>
+        <v>273.41326170779632</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1885,7 +1908,7 @@
       </c>
       <c r="F25" s="16">
         <f t="shared" si="1"/>
-        <v>223.45963572305229</v>
+        <v>223.52626493767727</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1899,7 +1922,7 @@
       </c>
       <c r="F26" s="16">
         <f t="shared" si="1"/>
-        <v>182.74009978934291</v>
+        <v>182.80144531114044</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1913,7 +1936,7 @@
       </c>
       <c r="F27" s="16">
         <f t="shared" si="1"/>
-        <v>149.49393372788859</v>
+        <v>149.55030041905593</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1927,7 +1950,7 @@
       </c>
       <c r="F28" s="16">
         <f t="shared" si="1"/>
-        <v>122.34435920698147</v>
+        <v>122.39605976712539</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1941,7 +1964,7 @@
       </c>
       <c r="F29" s="16">
         <f t="shared" si="1"/>
-        <v>100.16873194777504</v>
+        <v>100.21607932965509</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1955,7 +1978,7 @@
       </c>
       <c r="F30" s="16">
         <f t="shared" si="1"/>
-        <v>82.051584402107352</v>
+        <v>82.094886216185998</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1969,7 +1992,7 @@
       </c>
       <c r="F31" s="16">
         <f t="shared" si="1"/>
-        <v>67.246349482392034</v>
+        <v>67.285903966351853</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1983,7 +2006,7 @@
       </c>
       <c r="F32" s="16">
         <f t="shared" si="1"/>
-        <v>55.144160031136281</v>
+        <v>55.180253244268989</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1997,7 +2020,7 @@
       </c>
       <c r="F33" s="16">
         <f t="shared" si="1"/>
-        <v>45.248415616031707</v>
+        <v>45.281319586147191</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2011,7 +2034,7 @@
       </c>
       <c r="F34" s="16">
         <f t="shared" si="1"/>
-        <v>37.154050220374373</v>
+        <v>37.184021825628712</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2025,7 +2048,7 @@
       </c>
       <c r="F35" s="16">
         <f t="shared" si="1"/>
-        <v>30.530631625230761</v>
+        <v>30.55791203747793</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2039,7 +2062,7 @@
       </c>
       <c r="F36" s="16">
         <f t="shared" si="1"/>
-        <v>25.108584027872144</v>
+        <v>25.133398579795234</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2053,7 +2076,7 @@
       </c>
       <c r="F37" s="16">
         <f t="shared" si="1"/>
-        <v>20.667956457845957</v>
+        <v>20.690514824838317</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2067,7 +2090,7 @@
       </c>
       <c r="F38" s="16">
         <f t="shared" si="1"/>
-        <v>17.029266336881719</v>
+        <v>17.049762947742813</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2081,7 +2104,7 @@
       </c>
       <c r="F39" s="16">
         <f t="shared" si="1"/>
-        <v>14.046034563693896</v>
+        <v>14.064649172747496</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2095,7 +2118,7 @@
       </c>
       <c r="F40" s="16">
         <f t="shared" si="1"/>
-        <v>11.598699442648041</v>
+        <v>11.61559781075051</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2109,7 +2132,7 @@
       </c>
       <c r="F41" s="16">
         <f t="shared" si="1"/>
-        <v>9.5896545935188087</v>
+        <v>9.6049892373078212</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2123,7 +2146,7 @@
       </c>
       <c r="F42" s="16">
         <f t="shared" si="1"/>
-        <v>7.9392031047933047</v>
+        <v>7.9531140830053122</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2137,7 +2160,7 @@
       </c>
       <c r="F43" s="16">
         <f t="shared" si="1"/>
-        <v>6.5822586029264745</v>
+        <v>6.5948743161487071</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2151,7 +2174,7 @@
       </c>
       <c r="F44" s="16">
         <f t="shared" si="1"/>
-        <v>5.4656552165804628</v>
+        <v>5.4770932027774935</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2165,7 +2188,7 @@
       </c>
       <c r="F45" s="16">
         <f t="shared" si="1"/>
-        <v>4.5459539319677962</v>
+        <v>4.5563216448386665</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2179,7 +2202,7 @@
       </c>
       <c r="F46" s="16">
         <f t="shared" si="1"/>
-        <v>3.7876536337545681</v>
+        <v>3.7970491946817164</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2193,7 +2216,7 @@
       </c>
       <c r="F47" s="16">
         <f t="shared" si="1"/>
-        <v>3.161732078294746</v>
+        <v>3.1702449955406626</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2207,7 +2230,7 @@
       </c>
       <c r="F48" s="16">
         <f t="shared" si="1"/>
-        <v>2.6444558635683988</v>
+        <v>2.6521677146218905</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2221,7 +2244,7 @@
       </c>
       <c r="F49" s="16">
         <f t="shared" si="1"/>
-        <v>2.216409722829594</v>
+        <v>2.2233947975316339</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2235,7 +2258,7 @@
       </c>
       <c r="F50" s="16">
         <f t="shared" si="1"/>
-        <v>1.8617046491493627</v>
+        <v>1.8680305525442984</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2249,7 +2272,7 @@
       </c>
       <c r="F51" s="16">
         <f t="shared" si="1"/>
-        <v>1.5673318408862686</v>
+        <v>1.5730600557327503</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2263,7 +2286,7 @@
       </c>
       <c r="F52" s="16">
         <f t="shared" si="1"/>
-        <v>1.32263555752216</v>
+        <v>1.3278219671281004</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2277,7 +2300,7 @@
       </c>
       <c r="F53" s="16">
         <f t="shared" si="1"/>
-        <v>1.1188829470994219</v>
+        <v>1.12357831967165</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2291,7 +2314,7 @@
       </c>
       <c r="F54" s="16">
         <f t="shared" si="1"/>
-        <v>0.94891295920724683</v>
+        <v>0.95316339527351701</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2305,7 +2328,7 @@
       </c>
       <c r="F55" s="16">
         <f t="shared" si="1"/>
-        <v>0.806849761041872</v>
+        <v>0.81069710574590004</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2319,7 +2342,7 @@
       </c>
       <c r="F56" s="16">
         <f t="shared" si="1"/>
-        <v>0.68786876703118738</v>
+        <v>0.69135098924872385</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2333,7 +2356,7 @@
       </c>
       <c r="F57" s="16">
         <f t="shared" si="1"/>
-        <v>0.58800558777091261</v>
+        <v>0.59115712806906529</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2347,7 +2370,7 @@
       </c>
       <c r="F58" s="16">
         <f t="shared" si="1"/>
-        <v>0.50399999359108238</v>
+        <v>0.50685208307206475</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2361,7 +2384,7 @@
       </c>
       <c r="F59" s="16">
         <f t="shared" si="1"/>
-        <v>0.43316844696296092</v>
+        <v>0.43574939901137455</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2375,7 +2398,7 @@
       </c>
       <c r="F60" s="16">
         <f t="shared" si="1"/>
-        <v>0.37329994730232258</v>
+        <v>0.37563542420313017</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2389,7 +2412,7 @@
       </c>
       <c r="F61" s="16">
         <f t="shared" si="1"/>
-        <v>0.3225709013546047</v>
+        <v>0.32468415767590642</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2403,7 +2426,7 @@
       </c>
       <c r="F62" s="16">
         <f t="shared" si="1"/>
-        <v>0.27947552287576627</v>
+        <v>0.28138762742318024</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2417,7 +2440,7 @@
       </c>
       <c r="F63" s="16">
         <f t="shared" si="1"/>
-        <v>0.24276890985459815</v>
+        <v>0.24449894790775861</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2431,7 +2454,7 @@
       </c>
       <c r="F64" s="16">
         <f t="shared" si="1"/>
-        <v>0.21142047304130335</v>
+        <v>0.21298573048179242</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2445,7 +2468,7 @@
       </c>
       <c r="F65" s="16">
         <f t="shared" si="1"/>
-        <v>0.18457581804780607</v>
+        <v>0.18599194888479939</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2459,7 +2482,7 @@
       </c>
       <c r="F66" s="16">
         <f t="shared" si="1"/>
-        <v>0.16152553269536163</v>
+        <v>0.16280671139270356</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2473,7 +2496,7 @@
       </c>
       <c r="F67" s="16">
         <f t="shared" si="1"/>
-        <v>0.14167961621802541</v>
+        <v>0.14283867612603821</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2487,7 +2510,7 @@
       </c>
       <c r="F68" s="16">
         <f t="shared" si="1"/>
-        <v>0.1245465192982609</v>
+        <v>0.1255950783965489</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2501,7 +2524,7 @@
       </c>
       <c r="F69" s="16">
         <f t="shared" si="1"/>
-        <v>0.10971595342329599</v>
+        <v>0.11066452848795306</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2515,7 +2538,7 @@
       </c>
       <c r="F70" s="16">
         <f t="shared" si="1"/>
-        <v>9.6844782622840131E-2</v>
+        <v>9.7702892843351277E-2</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2529,7 +2552,7 @@
       </c>
       <c r="F71" s="16">
         <f t="shared" si="1"/>
-        <v>8.5645436732585067E-2</v>
+        <v>8.6421697720639234E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>